<commit_message>
approaching missing mail OK
</commit_message>
<xml_diff>
--- a/src/main/resources/Facebook-MissingMailQUESTION.xlsx
+++ b/src/main/resources/Facebook-MissingMailQUESTION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pessoal\Projects\playground\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67F808AB-46B6-4E9F-87C3-846D242A2E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4322E0BE-9211-42ED-829F-6599768429A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4680" yWindow="-1695" windowWidth="9285" windowHeight="8550" xr2:uid="{C2F41B1B-2AC8-4D77-B10D-4E01DBCC5F20}"/>
   </bookViews>
@@ -34,7 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23AA84B-8D6B-43A5-B6F5-329ECB510D88}">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -758,9 +765,335 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <f>0.85 *( 2 + 0.85 * 10)</f>
-        <v>8.9249999999999989</v>
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <f>MAX(B27+B35,C27)</f>
+        <v>2</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <f>MAX(D28,$B$28+C36)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" ref="B28:C28" si="4">MAX(C37+$B$29,D29)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <f>MAX(D37+$B$29,E29)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" ref="B29:D29" si="5">MAX(D30,C38+$B$30)</f>
+        <v>-2</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="5"/>
+        <v>-2</v>
+      </c>
+      <c r="E29" s="2">
+        <f>MAX(F30,E38+$B$30)</f>
+        <v>-2</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="1">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2">
+        <f>MAX(B39,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <f>C39</f>
+        <v>-4</v>
+      </c>
+      <c r="D30" s="2">
+        <f>D39</f>
+        <v>-4</v>
+      </c>
+      <c r="E30" s="2">
+        <f>E39</f>
+        <v>-4</v>
+      </c>
+      <c r="F30" s="2">
+        <f>F39</f>
+        <v>-4</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A34" s="1">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2">
+        <f>C35-$A$23</f>
+        <v>2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>10</v>
+      </c>
+      <c r="D35" s="2">
+        <f>C35*(1-$B$23)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" ref="E35:G38" si="6">D35*(1-$B$23)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A36" s="1">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2">
+        <f>D36-A23</f>
+        <v>-6</v>
+      </c>
+      <c r="C36" s="2">
+        <f>B36+D35</f>
+        <v>-6</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A37" s="1">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2">
+        <f>E37-A23</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <f>B37+E36</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f>C37+E35</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>8</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A38" s="1">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2">
+        <f>F38-A23</f>
+        <v>-2</v>
+      </c>
+      <c r="C38" s="2">
+        <f>B38+F37</f>
+        <v>-2</v>
+      </c>
+      <c r="D38" s="2">
+        <f>C38+F36</f>
+        <v>-2</v>
+      </c>
+      <c r="E38" s="2">
+        <f>D38+F35</f>
+        <v>-2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A39" s="1">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3">
+        <f>G39-$A$23</f>
+        <v>-4</v>
+      </c>
+      <c r="C39" s="3">
+        <f>B39+G38</f>
+        <v>-4</v>
+      </c>
+      <c r="D39" s="3">
+        <f>C39+G37</f>
+        <v>-4</v>
+      </c>
+      <c r="E39" s="3">
+        <f>D39+G36</f>
+        <v>-4</v>
+      </c>
+      <c r="F39" s="3">
+        <f>E39+G35</f>
+        <v>-4</v>
+      </c>
+      <c r="G39" s="3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>